<commit_message>
Agregando un nuevo permiso
</commit_message>
<xml_diff>
--- a/storage/app/utils/Permissions.xlsx
+++ b/storage/app/utils/Permissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crm.atalaya\storage\app\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1AADAF-E377-49FF-AFF8-95B9C248EBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E62EAFE-1C5F-4DD7-8FB5-E7B1D7D587DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>name</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>dashboard.list</t>
+  </si>
+  <si>
+    <t>Permite visualizar la pantalla de dashboard</t>
   </si>
 </sst>
 </file>
@@ -693,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1313F201-150F-4349-81B7-2BFCC09F2BD3}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,6 +1339,17 @@
         <v>111</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SOlo se puede ver sus proyectos
</commit_message>
<xml_diff>
--- a/storage/app/utils/Permissions.xlsx
+++ b/storage/app/utils/Permissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crm.atalaya\storage\app\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C99607-E738-4DAB-A606-DEC07A4D30E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CFB5DB-C4BF-4FCD-950D-22286B126754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>name</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>El usuario podrá eliminar ventanas de proyectos</t>
+  </si>
+  <si>
+    <t>projects.listall</t>
+  </si>
+  <si>
+    <t>El usuario podrá listar todos los proyectos. Si esta desactivado, solo puede ver sus asignados.</t>
   </si>
 </sst>
 </file>
@@ -749,15 +755,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1313F201-150F-4349-81B7-2BFCC09F2BD3}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A66"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1493,15 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>

</xml_diff>